<commit_message>
Fix titles - sential schemes
</commit_message>
<xml_diff>
--- a/data/SARI+USISS.xlsx
+++ b/data/SARI+USISS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\flu-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E8658E-DFB9-4A76-987A-61EEDEA5F924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C66FE8-BE66-4AE4-B4BC-1A402B5614C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="7" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -3730,6 +3730,7 @@
               <a:rPr lang="en-GB"/>
               <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) </a:t>
             </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6676,8 +6677,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) senti</a:t>
+              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>senti</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -15686,7 +15694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884B146F-6BB1-4927-ABB9-BD1C4945D1E8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -15731,7 +15739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC300B0-C4A3-42DB-A9B1-C2DB2BD92342}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add week 47 report (week 46 data)
</commit_message>
<xml_diff>
--- a/data/SARI+USISS.xlsx
+++ b/data/SARI+USISS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\flu-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E1D29D-007A-4ED3-8EE4-397E42B15525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AB119-2D3B-4EFD-9E00-1B5A66C36C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -632,13 +632,16 @@
                   <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.43</c:v>
+                  <c:v>10.44</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.53</c:v>
+                  <c:v>13.54</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.03</c:v>
+                  <c:v>14.23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.739999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,6 +1680,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,7 +2338,10 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.97</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3370,6 +3379,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4023,6 +4035,9 @@
                 <c:pt idx="18">
                   <c:v>26.53</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4124,6 +4139,9 @@
                 <c:pt idx="18">
                   <c:v>23.08</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.41</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4370,6 +4388,9 @@
                 <c:pt idx="18">
                   <c:v>19.55</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.64</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4616,6 +4637,9 @@
                 <c:pt idx="18">
                   <c:v>20.85</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.64</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4710,10 +4734,13 @@
                   <c:v>11.41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.149999999999999</c:v>
+                  <c:v>18.170000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.77</c:v>
+                  <c:v>17.71</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4963,6 +4990,9 @@
                 <c:pt idx="18">
                   <c:v>12.04</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.47</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5201,13 +5231,16 @@
                   <c:v>3.44</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.97</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.2799999999999994</c:v>
+                  <c:v>8.34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.05</c:v>
+                  <c:v>7.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5453,7 +5486,10 @@
                   <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.73</c:v>
+                  <c:v>7.79</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5702,6 +5738,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.08</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.9600000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7199,6 +7238,9 @@
                 <c:pt idx="18">
                   <c:v>1.65</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7296,7 +7338,10 @@
                   <c:v>1.61</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5</c:v>
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7543,6 +7588,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7645,6 +7693,9 @@
                 <c:pt idx="18">
                   <c:v>1.25</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.45</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7886,10 +7937,13 @@
                   <c:v>1.1299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.93</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.87</c:v>
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8135,7 +8189,10 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.91</c:v>
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8382,6 +8439,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8631,6 +8691,9 @@
                 <c:pt idx="18">
                   <c:v>0.52</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.66</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8878,6 +8941,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12734,11 +12800,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D77D55-EEF8-4CB5-9F33-DFA087C8AE95}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12990,7 +13056,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="2">
-        <v>10.43</v>
+        <v>10.44</v>
       </c>
       <c r="C18" s="2">
         <v>0.03</v>
@@ -13011,7 +13077,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="2">
-        <v>13.53</v>
+        <v>13.54</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -13032,7 +13098,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>14.03</v>
+        <v>14.23</v>
       </c>
       <c r="C20" s="2">
         <v>0.01</v>
@@ -13052,8 +13118,12 @@
       <c r="A21" s="1">
         <v>46</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="2">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
       <c r="D21" s="4">
         <v>1.3588927825232173</v>
       </c>
@@ -13546,10 +13616,10 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15:C20"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13838,7 +13908,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -13857,8 +13927,12 @@
       <c r="A21" s="1">
         <v>46</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
       <c r="D21" s="4">
         <v>5.3697774503406813E-2</v>
       </c>
@@ -14326,7 +14400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14889,7 +14963,7 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="D18" s="3">
-        <v>5.97</v>
+        <v>6</v>
       </c>
       <c r="E18" s="3">
         <v>17.440000000000001</v>
@@ -14921,7 +14995,7 @@
         <v>7.25</v>
       </c>
       <c r="D19" s="3">
-        <v>8.2799999999999994</v>
+        <v>8.34</v>
       </c>
       <c r="E19" s="3">
         <v>24.43</v>
@@ -14936,7 +15010,7 @@
         <v>7.52</v>
       </c>
       <c r="I19" s="4">
-        <v>18.149999999999999</v>
+        <v>18.170000000000002</v>
       </c>
       <c r="J19" s="4">
         <v>21.96</v>
@@ -14950,10 +15024,10 @@
         <v>20.85</v>
       </c>
       <c r="C20" s="3">
-        <v>7.73</v>
+        <v>7.79</v>
       </c>
       <c r="D20" s="3">
-        <v>7.05</v>
+        <v>7.02</v>
       </c>
       <c r="E20" s="3">
         <v>26.53</v>
@@ -14968,7 +15042,7 @@
         <v>12.04</v>
       </c>
       <c r="I20" s="4">
-        <v>15.77</v>
+        <v>17.71</v>
       </c>
       <c r="J20" s="4">
         <v>23.08</v>
@@ -14978,15 +15052,33 @@
       <c r="A21" s="1">
         <v>46</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="B21" s="3">
+        <v>24.64</v>
+      </c>
+      <c r="C21" s="3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="E21" s="3">
+        <v>26.1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>20.64</v>
+      </c>
+      <c r="G21" s="3">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="H21" s="4">
+        <v>15.47</v>
+      </c>
+      <c r="I21" s="4">
+        <v>21.05</v>
+      </c>
+      <c r="J21" s="4">
+        <v>29.41</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -15414,7 +15506,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16015,7 +16107,7 @@
         <v>0.92</v>
       </c>
       <c r="F19" s="3">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="G19" s="3">
         <v>0.3</v>
@@ -16041,13 +16133,13 @@
         <v>0.75</v>
       </c>
       <c r="D20" s="3">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="E20" s="3">
         <v>1.44</v>
       </c>
       <c r="F20" s="3">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="G20" s="3">
         <v>0.43</v>
@@ -16056,7 +16148,7 @@
         <v>0.52</v>
       </c>
       <c r="I20" s="4">
-        <v>1.5</v>
+        <v>1.79</v>
       </c>
       <c r="J20" s="4">
         <v>1.25</v>
@@ -16066,15 +16158,33 @@
       <c r="A21" s="1">
         <v>46</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="B21" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.26</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.32</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1.45</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -16545,7 +16655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC300B0-C4A3-42DB-A9B1-C2DB2BD92342}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add week 48 report (week 47 data)
</commit_message>
<xml_diff>
--- a/data/SARI+USISS.xlsx
+++ b/data/SARI+USISS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\flu-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AB119-2D3B-4EFD-9E00-1B5A66C36C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF28263-50E8-4B79-B5A5-1575956E6CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="6" xr2:uid="{D71F1701-F75D-44F5-9C73-75EE478BE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Week 45 figures are likely to rise due to a lag in the data reporting</a:t>
+              <a:t>Week 47 figures are likely to rise slightly due to a lag in the data reporting</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -363,7 +363,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) </a:t>
+              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infectio</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -584,64 +584,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v>1.4452523834307971</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.24</c:v>
+                  <c:v>1.2394281712766009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.01</c:v>
+                  <c:v>1.0075809951179933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77</c:v>
+                  <c:v>0.77366653695374987</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77</c:v>
+                  <c:v>0.76604878933380549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69</c:v>
+                  <c:v>0.68631605384305738</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67</c:v>
+                  <c:v>0.67433237656512213</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.56510281897079906</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53</c:v>
+                  <c:v>0.53058170558002538</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76</c:v>
+                  <c:v>0.7565283497377695</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.39</c:v>
+                  <c:v>1.3879719044153385</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.12</c:v>
+                  <c:v>2.1211056349355011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.02</c:v>
+                  <c:v>3.0220041181390238</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.57</c:v>
+                  <c:v>3.5697235519542616</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.51</c:v>
+                  <c:v>5.5088076763559757</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.6</c:v>
+                  <c:v>7.6028365483897051</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.44</c:v>
+                  <c:v>10.431488054298061</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.54</c:v>
+                  <c:v>13.543695015386776</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.23</c:v>
+                  <c:v>14.236911325106819</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16.739999999999998</c:v>
+                  <c:v>16.875102593700198</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.500965072717902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1664,25 +1667,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="13">
-                  <c:v>0.01</c:v>
+                  <c:v>9.7427087029473454E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.03</c:v>
+                  <c:v>2.5133014384210572E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05</c:v>
+                  <c:v>5.2289832782343747E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>2.5806715784875558E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9489798968325797E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0220025965046311E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,7 +2060,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Week 45 figures are likely to rise due to a lag in the data reporting</a:t>
+              <a:t>Week 47 figures are likely to rise </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>slightly </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>due to a lag in the data reporting</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2063,7 +2079,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) senti</a:t>
+              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SA</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2284,64 +2300,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.11</c:v>
+                  <c:v>0.10766977950142011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11</c:v>
+                  <c:v>0.10913766763636697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.3776320951937299E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.2051707466255915E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.08</c:v>
+                  <c:v>8.034852543559004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.8855804809084098E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.05</c:v>
+                  <c:v>5.1034484803352098E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>8.4253098329456044E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9155562648107669E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.6190317018523362E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13</c:v>
+                  <c:v>0.13007717218471374</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25</c:v>
+                  <c:v>0.24957189673032129</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.38</c:v>
+                  <c:v>0.38313056946133278</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4</c:v>
+                  <c:v>0.40485929068275656</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.48</c:v>
+                  <c:v>0.47507031099108865</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58222436145913092</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.73</c:v>
+                  <c:v>0.73030003919276876</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91971937400412318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>1.0032415900250555</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.05</c:v>
+                  <c:v>1.0562139034815183</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.96053415348951565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3367,13 +3386,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>4.4905763347121118E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>4.1712603540328026E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2.1707387627475008E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -3382,6 +3401,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>4.13334962975314E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3750,7 +3772,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Week 45 figures are likely to rise due to a lag in the data reporting</a:t>
+              <a:t>Week 47 figures are likely to rise </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>slightly </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>due to a lag in the data reporting</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -3759,7 +3791,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) </a:t>
+              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infectio</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3979,64 +4011,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.74</c:v>
+                  <c:v>0.74213200807571411</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93</c:v>
+                  <c:v>0.92766499519348145</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31</c:v>
+                  <c:v>0.30922168493270874</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42</c:v>
+                  <c:v>0.42372414469718933</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17</c:v>
+                  <c:v>0.16948965191841125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59</c:v>
+                  <c:v>0.59321379661560059</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.37</c:v>
+                  <c:v>0.37106600403785706</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25</c:v>
+                  <c:v>0.24737733602523804</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25</c:v>
+                  <c:v>0.24737733602523804</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>1.1131980419158936</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.23</c:v>
+                  <c:v>2.2263960838317871</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3899999999999997</c:v>
+                  <c:v>4.3909478187561035</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.79</c:v>
+                  <c:v>7.7923860549926758</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.76</c:v>
+                  <c:v>10.760913848876953</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.25</c:v>
+                  <c:v>12.24517822265625</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.88</c:v>
+                  <c:v>16.883502960205078</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.440000000000001</c:v>
+                  <c:v>17.440101623535156</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.43</c:v>
+                  <c:v>24.428512573242188</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.53</c:v>
+                  <c:v>26.531219482421875</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26.1</c:v>
+                  <c:v>26.098308563232422</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30.056346893310547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4083,64 +4118,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.93</c:v>
+                  <c:v>1.9267857074737549</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.26</c:v>
+                  <c:v>1.258309006690979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.51</c:v>
+                  <c:v>1.513903021812439</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77</c:v>
+                  <c:v>0.76678204536437988</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.87</c:v>
+                  <c:v>0.86508744955062866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94</c:v>
+                  <c:v>0.94373178482055664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83</c:v>
+                  <c:v>0.82576531171798706</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.56818699836730957</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.5701712965965271</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51</c:v>
+                  <c:v>0.50730985403060913</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.06</c:v>
+                  <c:v>1.0616981983184814</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.95</c:v>
+                  <c:v>2.9491617679595947</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.25</c:v>
+                  <c:v>4.2467927932739258</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.45</c:v>
+                  <c:v>5.4461188316345215</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.73</c:v>
+                  <c:v>8.7300834655761719</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.91</c:v>
+                  <c:v>11.909671783447266</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.010000000000002</c:v>
+                  <c:v>18.011541366577148</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.96</c:v>
+                  <c:v>21.963052749633789</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.08</c:v>
+                  <c:v>23.084178924560547</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.41</c:v>
+                  <c:v>29.406597137451172</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.882007598876953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4332,64 +4370,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>2.4</c:v>
+                  <c:v>2.3968398571014404</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.14</c:v>
+                  <c:v>2.1430132389068604</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.77</c:v>
+                  <c:v>1.7652401924133301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.57</c:v>
+                  <c:v>1.5709018707275391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.72</c:v>
+                  <c:v>1.7237280607223511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.48</c:v>
+                  <c:v>1.4752627611160278</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.58</c:v>
+                  <c:v>1.5839662551879883</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.26</c:v>
+                  <c:v>1.2556016445159912</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.42</c:v>
+                  <c:v>1.4205218553543091</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.88</c:v>
+                  <c:v>1.884222149848938</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.59</c:v>
+                  <c:v>2.5933566093444824</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.18</c:v>
+                  <c:v>4.1773228645324707</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.33</c:v>
+                  <c:v>5.326474666595459</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.11</c:v>
+                  <c:v>7.1123189926147461</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.05</c:v>
+                  <c:v>12.050566673278809</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.43</c:v>
+                  <c:v>16.429767608642578</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.350000000000001</c:v>
+                  <c:v>19.349235534667969</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.94</c:v>
+                  <c:v>21.942592620849609</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.55</c:v>
+                  <c:v>19.551113128662109</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.64</c:v>
+                  <c:v>20.638149261474609</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.876859664916992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4581,64 +4622,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.97</c:v>
+                  <c:v>1.9703766107559204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3</c:v>
+                  <c:v>1.2975651025772095</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>1.1053332090377808</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.57669556140899658</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46</c:v>
+                  <c:v>0.45655068755149841</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.44</c:v>
+                  <c:v>0.44457253813743591</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46</c:v>
+                  <c:v>0.45655068755149841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.66</c:v>
+                  <c:v>0.65857481956481934</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76</c:v>
+                  <c:v>0.75608879327774048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0.5046086311340332</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.89</c:v>
+                  <c:v>1.8934025764465332</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.32</c:v>
+                  <c:v>1.3215939998626709</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.21</c:v>
+                  <c:v>2.2106664180755615</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.67</c:v>
+                  <c:v>2.6672170162200928</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.5599999999999996</c:v>
+                  <c:v>4.5551424026489258</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.67</c:v>
+                  <c:v>8.6712350845336914</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.88</c:v>
+                  <c:v>13.884951591491699</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.52</c:v>
+                  <c:v>16.519250869750977</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.85</c:v>
+                  <c:v>20.854867935180664</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.64</c:v>
+                  <c:v>24.66911506652832</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.45539665222168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4683,64 +4727,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.93</c:v>
+                  <c:v>0.92778003215789795</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.36</c:v>
+                  <c:v>1.3577268123626709</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78</c:v>
+                  <c:v>0.7753746509552002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84</c:v>
+                  <c:v>0.83553707599639893</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86</c:v>
+                  <c:v>0.85989367961883545</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81</c:v>
+                  <c:v>0.81463611125946045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84</c:v>
+                  <c:v>0.83726489543914795</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.54</c:v>
+                  <c:v>0.54309076070785522</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                  <c:v>0.74674975872039795</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.35</c:v>
+                  <c:v>1.3528138399124146</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.44</c:v>
+                  <c:v>2.4436049461364746</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.67</c:v>
+                  <c:v>3.6658625602722168</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.45</c:v>
+                  <c:v>5.4535360336303711</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5</c:v>
+                  <c:v>5.4987936019897461</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.36</c:v>
+                  <c:v>6.3612508773803711</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.83</c:v>
+                  <c:v>7.8343825340270996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.41</c:v>
+                  <c:v>11.405611038208008</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.170000000000002</c:v>
+                  <c:v>18.168624877929688</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.71</c:v>
+                  <c:v>17.713386535644531</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.05</c:v>
+                  <c:v>21.762172698974609</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.832464218139648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4934,64 +4981,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.3978596031665802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42</c:v>
+                  <c:v>0.41879957914352417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31</c:v>
+                  <c:v>0.31409966945648193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19</c:v>
+                  <c:v>0.18845981359481812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42</c:v>
+                  <c:v>0.41879957914352417</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35</c:v>
+                  <c:v>0.34651708602905273</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36</c:v>
+                  <c:v>0.35597965121269226</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.49811831116676331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>8.3759918808937073E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19</c:v>
+                  <c:v>0.19491586089134216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23823049664497375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.54</c:v>
+                  <c:v>0.54143291711807251</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.73</c:v>
+                  <c:v>0.7328992486000061</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95</c:v>
+                  <c:v>0.95292198657989502</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7</c:v>
+                  <c:v>1.6961382627487183</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.06</c:v>
+                  <c:v>3.057236909866333</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.59</c:v>
+                  <c:v>4.5862536430358887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.52</c:v>
+                  <c:v>7.515289306640625</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12.04</c:v>
+                  <c:v>12.043732643127441</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.47</c:v>
+                  <c:v>15.473788261413574</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16.861225128173828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5183,64 +5233,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.27</c:v>
+                  <c:v>1.2652630805969238</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.19</c:v>
+                  <c:v>1.1853517293930054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73</c:v>
+                  <c:v>0.7325206995010376</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77</c:v>
+                  <c:v>0.77247637510299683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46</c:v>
+                  <c:v>0.4617595374584198</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34</c:v>
+                  <c:v>0.335825115442276</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.44776681065559387</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.37</c:v>
+                  <c:v>0.37313216924667358</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.29021391272544861</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55315732955932617</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>1.0044173002243042</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.81</c:v>
+                  <c:v>1.805039644241333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4300000000000002</c:v>
+                  <c:v>2.430980920791626</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.78</c:v>
+                  <c:v>1.7770745754241943</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.81</c:v>
+                  <c:v>2.8088922500610352</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.44</c:v>
+                  <c:v>3.4353981018066406</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>5.9682765007019043</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.34</c:v>
+                  <c:v>8.3410301208496094</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.02</c:v>
+                  <c:v>7.0243420600891113</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.78</c:v>
+                  <c:v>8.0458097457885742</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.682635307312012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5432,64 +5485,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.38</c:v>
+                  <c:v>1.3844501972198486</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97</c:v>
+                  <c:v>0.96547180414199829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87</c:v>
+                  <c:v>0.87438958883285522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87</c:v>
+                  <c:v>0.87438958883285522</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77</c:v>
+                  <c:v>0.76509088277816772</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58292639255523682</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47</c:v>
+                  <c:v>0.47362768650054932</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4</c:v>
+                  <c:v>0.40076187252998352</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26</c:v>
+                  <c:v>0.25520727038383484</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38</c:v>
+                  <c:v>0.38254544138908386</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.95</c:v>
+                  <c:v>0.9523242712020874</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.93</c:v>
+                  <c:v>0.92903894186019897</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.06</c:v>
+                  <c:v>1.0565540790557861</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.68</c:v>
+                  <c:v>1.6804071664810181</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3199999999999998</c:v>
+                  <c:v>2.3202061653137207</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.62</c:v>
+                  <c:v>3.6225960254669189</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.4800000000000004</c:v>
+                  <c:v>4.4798507690429688</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.25</c:v>
+                  <c:v>7.251431941986084</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.79</c:v>
+                  <c:v>7.8111362457275391</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.7100000000000009</c:v>
+                  <c:v>9.8661308288574219</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.6569547653198242</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5683,64 +5739,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>1.38</c:v>
+                  <c:v>1.3796178102493286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.18</c:v>
+                  <c:v>1.1825294494628906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.1004093885421753</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49</c:v>
+                  <c:v>0.48768395185470581</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55495071411132813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                  <c:v>0.47086727619171143</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39</c:v>
+                  <c:v>0.38678383827209473</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>0.33305755257606506</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35</c:v>
+                  <c:v>0.35315045714378357</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44</c:v>
+                  <c:v>0.43823361396789551</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.77</c:v>
+                  <c:v>0.77356767654418945</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.67</c:v>
+                  <c:v>0.67266756296157837</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.28</c:v>
+                  <c:v>1.2780683040618896</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1299999999999999</c:v>
+                  <c:v>1.1267181634902954</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.33</c:v>
+                  <c:v>2.3322110176086426</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.04</c:v>
+                  <c:v>3.0384438037872314</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.21</c:v>
+                  <c:v>5.2064146995544434</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.82</c:v>
+                  <c:v>5.8185739517211914</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.08</c:v>
+                  <c:v>7.0798258781433105</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9600000000000009</c:v>
+                  <c:v>8.9632949829101563</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.7032289505004883</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6784,7 +6843,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6946,7 +7005,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Week 45 figures are likely to rise due to a lag in the data reporting</a:t>
+              <a:t>Week 47 figures are likely to rise </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>slightly </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>due to a lag in the data reporting</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -6955,13 +7024,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SARI) </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>senti</a:t>
+              <a:t>Sources: UK Severe Influenza Surveillance Systems (USISS) and Severe Acute Respiratory Infection (SA</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -7182,64 +7245,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.13</c:v>
+                  <c:v>0.13075663149356842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>5.2302651107311249E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15</c:v>
+                  <c:v>0.1512177586555481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>2.402898296713829E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.05</c:v>
+                  <c:v>5.4881233721971512E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0487102717161179E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12</c:v>
+                  <c:v>0.12097420543432236</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>0.1046053022146225</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0487102717161179E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19</c:v>
+                  <c:v>0.19208431243896484</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16</c:v>
+                  <c:v>0.15690794587135315</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.33</c:v>
+                  <c:v>0.33267906308174133</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11</c:v>
+                  <c:v>0.10976246744394302</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.45</c:v>
+                  <c:v>0.45365327596664429</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.57462745904922485</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.91</c:v>
+                  <c:v>0.9055403470993042</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.45</c:v>
+                  <c:v>1.4543526172637939</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.65</c:v>
+                  <c:v>1.6464369297027588</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.73</c:v>
+                  <c:v>1.7287588119506836</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7287588119506836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7284,64 +7350,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.23</c:v>
+                  <c:v>0.22964039444923401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.2041248083114624</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.14097721874713898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13</c:v>
+                  <c:v>0.1339210718870163</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16</c:v>
+                  <c:v>0.15840145945549011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>0.20365902781486511</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.7886345088481903E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.02</c:v>
+                  <c:v>2.2628780454397202E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>7.6546803116798401E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16</c:v>
+                  <c:v>0.16327063739299774</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.26</c:v>
+                  <c:v>0.25845822691917419</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.61</c:v>
+                  <c:v>0.61097711324691772</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.06</c:v>
+                  <c:v>1.0635527372360229</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.86</c:v>
+                  <c:v>0.85989367961883545</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.69</c:v>
+                  <c:v>0.6919255256652832</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.89</c:v>
+                  <c:v>0.89280712604522705</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.32</c:v>
+                  <c:v>1.3168904781341553</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.61</c:v>
+                  <c:v>1.6070528030395508</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.79</c:v>
+                  <c:v>1.7856142520904541</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.52</c:v>
+                  <c:v>1.5177720785140991</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9238219261169434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7536,7 +7605,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.08</c:v>
+                  <c:v>8.4744825959205627E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -7557,40 +7626,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.05</c:v>
+                  <c:v>5.3836699575185776E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08</c:v>
+                  <c:v>8.4744825959205627E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.05</c:v>
+                  <c:v>5.3836699575185776E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48</c:v>
+                  <c:v>0.48453029990196228</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.48</c:v>
+                  <c:v>0.47942420840263367</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.61</c:v>
+                  <c:v>0.61017626523971558</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.44</c:v>
+                  <c:v>0.4358401894569397</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91526436805725098</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.7</c:v>
+                  <c:v>0.69734430313110352</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91526436805725098</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.44</c:v>
+                  <c:v>1.4382725954055786</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.26</c:v>
+                  <c:v>1.2639365196228027</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3511046171188354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7637,64 +7709,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0877177864313126E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.28409349918365479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.10146196186542511</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.13762754201889038</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0877177864313126E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0877177864313126E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.08</c:v>
+                  <c:v>7.8644312918186188E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>8.1169575452804565E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12</c:v>
+                  <c:v>0.12175435572862625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08</c:v>
+                  <c:v>8.1169575452804565E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16</c:v>
+                  <c:v>0.16233915090560913</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.27525508403778076</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.35</c:v>
+                  <c:v>0.35389941930770874</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.53</c:v>
+                  <c:v>0.53084909915924072</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91895616054534912</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87</c:v>
+                  <c:v>0.87076354026794434</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>1.1547081470489502</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.42</c:v>
+                  <c:v>1.4151924848556519</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.25</c:v>
+                  <c:v>1.2493563890457153</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.45</c:v>
+                  <c:v>1.4519506692886353</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.173637866973877</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7886,64 +7961,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.19</c:v>
+                  <c:v>0.19477562606334686</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1423524245619774E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14935484528541565</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13</c:v>
+                  <c:v>0.12955892086029053</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11775144934654236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17</c:v>
+                  <c:v>0.16821636259555817</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13</c:v>
+                  <c:v>0.12854114174842834</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17</c:v>
+                  <c:v>0.17151154577732086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.2847269475460052E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19</c:v>
+                  <c:v>0.1850380003452301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23819261789321899</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32</c:v>
+                  <c:v>0.3203335702419281</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.61</c:v>
+                  <c:v>0.60563415288925171</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.65</c:v>
+                  <c:v>0.64779460430145264</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.76</c:v>
+                  <c:v>0.76115864515304565</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.85</c:v>
+                  <c:v>0.85409945249557495</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1299999999999999</c:v>
+                  <c:v>1.1273124217987061</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.95</c:v>
+                  <c:v>0.94727396965026855</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.89</c:v>
+                  <c:v>0.88515764474868774</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.32</c:v>
+                  <c:v>1.335500955581665</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.55779355764389038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8135,64 +8213,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11986702680587769</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.14312003552913666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.04</c:v>
+                  <c:v>3.9955675601959229E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.10018402338027954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17</c:v>
+                  <c:v>0.1660277396440506</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.03</c:v>
+                  <c:v>2.7985425665974617E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.03</c:v>
+                  <c:v>2.7985425665974617E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11</c:v>
+                  <c:v>0.11194170266389847</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1</c:v>
+                  <c:v>9.6737965941429138E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.05</c:v>
+                  <c:v>4.7255426645278931E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15</c:v>
+                  <c:v>0.15211443603038788</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.36</c:v>
+                  <c:v>0.36391928791999817</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.45</c:v>
+                  <c:v>0.45125991106033325</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.33</c:v>
+                  <c:v>0.33436283469200134</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.32</c:v>
+                  <c:v>0.32335537672042847</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.49</c:v>
+                  <c:v>0.49493023753166199</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.66</c:v>
+                  <c:v>0.65505474805831909</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91707664728164673</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.92</c:v>
+                  <c:v>0.92269307374954224</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.63</c:v>
+                  <c:v>0.65765750408172607</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90952634811401367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8384,64 +8465,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>0.15705062448978424</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12</c:v>
+                  <c:v>0.12340131402015686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.06</c:v>
+                  <c:v>5.8893982321023941E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>1.963132806122303E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02</c:v>
+                  <c:v>1.963132806122303E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.04</c:v>
+                  <c:v>3.6432899534702301E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>9.8156638443470001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.04</c:v>
+                  <c:v>3.926265612244606E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.04</c:v>
+                  <c:v>4.4017631560564041E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>8.2267537713050842E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11</c:v>
+                  <c:v>0.1092986986041069</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.36</c:v>
+                  <c:v>0.3644256591796875</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.36</c:v>
+                  <c:v>0.35840582847595215</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.31</c:v>
+                  <c:v>0.3063887357711792</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33</c:v>
+                  <c:v>0.33119520545005798</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.63</c:v>
+                  <c:v>0.62752777338027954</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75</c:v>
+                  <c:v>0.74954706430435181</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.75</c:v>
+                  <c:v>0.74954706430435181</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76697838306427002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8638,34 +8722,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.02</c:v>
+                  <c:v>2.0939979702234268E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>2.0939979702234268E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.04</c:v>
+                  <c:v>4.1879959404468536E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.02</c:v>
+                  <c:v>2.0939979702234268E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.06</c:v>
+                  <c:v>6.4971953630447388E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.06</c:v>
+                  <c:v>6.2819935381412506E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1657317876815796E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1657317876815796E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -8674,25 +8758,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.04</c:v>
+                  <c:v>4.3314635753631592E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.15</c:v>
+                  <c:v>0.15160122513771057</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27</c:v>
+                  <c:v>0.27221971750259399</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.18</c:v>
+                  <c:v>0.17888219654560089</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.42</c:v>
+                  <c:v>0.41739180684089661</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.52</c:v>
+                  <c:v>0.52028924226760864</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.66</c:v>
+                  <c:v>0.65590143203735352</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.59736913442611694</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8886,31 +8973,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7103113234043121E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2848041504621506E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7103113234043121E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>1.9665028899908066E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02</c:v>
+                  <c:v>1.752934418618679E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02</c:v>
+                  <c:v>1.9665028899908066E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.02</c:v>
+                  <c:v>1.752934418618679E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.02</c:v>
+                  <c:v>1.9665028899908066E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.02</c:v>
+                  <c:v>1.8772562965750694E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -8919,31 +9006,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.06</c:v>
+                  <c:v>5.5492110550403595E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.09</c:v>
+                  <c:v>9.3862816691398621E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.17</c:v>
+                  <c:v>0.16895307600498199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.11</c:v>
+                  <c:v>0.10814039409160614</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.21</c:v>
+                  <c:v>0.20831501483917236</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.28695294260978699</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.3</c:v>
+                  <c:v>0.30270040035247803</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.43</c:v>
+                  <c:v>0.43263065814971924</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.65</c:v>
+                  <c:v>0.6485857367515564</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.57176738977432251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9987,7 +10077,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12800,11 +12890,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D77D55-EEF8-4CB5-9F33-DFA087C8AE95}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12837,7 +12927,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2">
-        <v>1.45</v>
+        <v>1.4452523834307971</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
@@ -12849,7 +12939,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>1.24</v>
+        <v>1.2394281712766009</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
@@ -12861,7 +12951,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2">
-        <v>1.01</v>
+        <v>1.0075809951179933</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -12873,7 +12963,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="2">
-        <v>0.77</v>
+        <v>0.77366653695374987</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
@@ -12885,7 +12975,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="2">
-        <v>0.77</v>
+        <v>0.76604878933380549</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -12897,7 +12987,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="2">
-        <v>0.69</v>
+        <v>0.68631605384305738</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
@@ -12909,7 +12999,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="2">
-        <v>0.67</v>
+        <v>0.67433237656512213</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
@@ -12921,7 +13011,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.56510281897079906</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
@@ -12933,7 +13023,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="2">
-        <v>0.53</v>
+        <v>0.53058170558002538</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
@@ -12945,7 +13035,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="2">
-        <v>0.76</v>
+        <v>0.7565283497377695</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
@@ -12957,7 +13047,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="2">
-        <v>1.39</v>
+        <v>1.3879719044153385</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -12969,7 +13059,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="2">
-        <v>2.12</v>
+        <v>2.1211056349355011</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
@@ -12981,7 +13071,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="2">
-        <v>3.02</v>
+        <v>3.0220041181390238</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
@@ -12993,10 +13083,10 @@
         <v>40</v>
       </c>
       <c r="B15" s="2">
-        <v>3.57</v>
+        <v>3.5697235519542616</v>
       </c>
       <c r="C15" s="2">
-        <v>0.01</v>
+        <v>9.7427087029473454E-3</v>
       </c>
       <c r="D15" s="4">
         <v>3.5616945450392304E-2</v>
@@ -13014,10 +13104,10 @@
         <v>41</v>
       </c>
       <c r="B16" s="2">
-        <v>5.51</v>
+        <v>5.5088076763559757</v>
       </c>
       <c r="C16" s="2">
-        <v>0.03</v>
+        <v>2.5133014384210572E-2</v>
       </c>
       <c r="D16" s="4">
         <v>0.29359339685866359</v>
@@ -13035,10 +13125,10 @@
         <v>42</v>
       </c>
       <c r="B17" s="2">
-        <v>7.6</v>
+        <v>7.6028365483897051</v>
       </c>
       <c r="C17" s="2">
-        <v>0.05</v>
+        <v>5.2289832782343747E-2</v>
       </c>
       <c r="D17" s="4">
         <v>0.22162802458931272</v>
@@ -13056,10 +13146,10 @@
         <v>43</v>
       </c>
       <c r="B18" s="2">
-        <v>10.44</v>
+        <v>10.431488054298061</v>
       </c>
       <c r="C18" s="2">
-        <v>0.03</v>
+        <v>2.5806715784875558E-2</v>
       </c>
       <c r="D18" s="4">
         <v>0.63036847401187768</v>
@@ -13077,7 +13167,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="2">
-        <v>13.54</v>
+        <v>13.543695015386776</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -13098,10 +13188,10 @@
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>14.23</v>
+        <v>14.236911325106819</v>
       </c>
       <c r="C20" s="2">
-        <v>0.01</v>
+        <v>8.9489798968325797E-3</v>
       </c>
       <c r="D20" s="4">
         <v>0.8246341208744048</v>
@@ -13119,7 +13209,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="2">
-        <v>16.739999999999998</v>
+        <v>16.875102593700198</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -13139,8 +13229,12 @@
       <c r="A22" s="1">
         <v>47</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2">
+        <v>15.500965072717902</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.0220025965046311E-2</v>
+      </c>
       <c r="D22" s="4">
         <v>2.8153170321395375</v>
       </c>
@@ -13619,7 +13713,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15:C21"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13652,7 +13746,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2">
-        <v>0.11</v>
+        <v>0.10766977950142011</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
@@ -13664,7 +13758,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>0.11</v>
+        <v>0.10913766763636697</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
@@ -13676,7 +13770,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.3776320951937299E-2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -13688,7 +13782,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2051707466255915E-2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
@@ -13700,7 +13794,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="2">
-        <v>0.08</v>
+        <v>8.034852543559004E-2</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -13712,7 +13806,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>6.8855804809084098E-2</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
@@ -13724,7 +13818,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="2">
-        <v>0.05</v>
+        <v>5.1034484803352098E-2</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
@@ -13736,7 +13830,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="2">
-        <v>0.08</v>
+        <v>8.4253098329456044E-2</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
@@ -13748,7 +13842,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9155562648107669E-2</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
@@ -13760,7 +13854,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6190317018523362E-2</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
@@ -13772,7 +13866,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="2">
-        <v>0.13</v>
+        <v>0.13007717218471374</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -13784,7 +13878,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="2">
-        <v>0.25</v>
+        <v>0.24957189673032129</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
@@ -13796,7 +13890,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="2">
-        <v>0.38</v>
+        <v>0.38313056946133278</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
@@ -13808,7 +13902,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="2">
-        <v>0.4</v>
+        <v>0.40485929068275656</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -13828,10 +13922,10 @@
         <v>41</v>
       </c>
       <c r="B16" s="2">
-        <v>0.48</v>
+        <v>0.47507031099108865</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>4.4905763347121118E-3</v>
       </c>
       <c r="D16" s="4">
         <v>1.5532863422793825E-2</v>
@@ -13848,10 +13942,10 @@
         <v>42</v>
       </c>
       <c r="B17" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.58222436145913092</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>4.1712603540328026E-3</v>
       </c>
       <c r="D17" s="4">
         <v>1.785312873700699E-2</v>
@@ -13868,10 +13962,10 @@
         <v>43</v>
       </c>
       <c r="B18" s="2">
-        <v>0.73</v>
+        <v>0.73030003919276876</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>2.1707387627475008E-3</v>
       </c>
       <c r="D18" s="4">
         <v>2.1264852363639567E-2</v>
@@ -13888,7 +13982,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="2">
-        <v>0.92</v>
+        <v>0.91971937400412318</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -13908,7 +14002,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>1.0032415900250555</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -13928,10 +14022,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="2">
-        <v>1.05</v>
+        <v>1.0562139034815183</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>4.13334962975314E-3</v>
       </c>
       <c r="D21" s="4">
         <v>5.3697774503406813E-2</v>
@@ -13947,8 +14041,12 @@
       <c r="A22" s="1">
         <v>47</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2">
+        <v>0.96053415348951565</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
       <c r="D22" s="4">
         <v>8.2464439415946181E-2</v>
       </c>
@@ -14400,7 +14498,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14445,31 +14543,31 @@
         <v>27</v>
       </c>
       <c r="B2" s="3">
-        <v>1.97</v>
+        <v>1.9703766107559204</v>
       </c>
       <c r="C2" s="3">
-        <v>1.38</v>
+        <v>1.3844501972198486</v>
       </c>
       <c r="D2" s="3">
-        <v>1.27</v>
+        <v>1.2652630805969238</v>
       </c>
       <c r="E2" s="3">
-        <v>0.74</v>
+        <v>0.74213200807571411</v>
       </c>
       <c r="F2" s="3">
-        <v>2.4</v>
+        <v>2.3968398571014404</v>
       </c>
       <c r="G2" s="3">
-        <v>1.38</v>
+        <v>1.3796178102493286</v>
       </c>
       <c r="H2" s="4">
-        <v>0.4</v>
+        <v>0.3978596031665802</v>
       </c>
       <c r="I2" s="4">
-        <v>0.93</v>
+        <v>0.92778003215789795</v>
       </c>
       <c r="J2" s="4">
-        <v>1.93</v>
+        <v>1.9267857074737549</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -14477,31 +14575,31 @@
         <v>28</v>
       </c>
       <c r="B3" s="3">
-        <v>1.3</v>
+        <v>1.2975651025772095</v>
       </c>
       <c r="C3" s="3">
-        <v>0.97</v>
+        <v>0.96547180414199829</v>
       </c>
       <c r="D3" s="3">
-        <v>1.19</v>
+        <v>1.1853517293930054</v>
       </c>
       <c r="E3" s="3">
-        <v>0.93</v>
+        <v>0.92766499519348145</v>
       </c>
       <c r="F3" s="3">
-        <v>2.14</v>
+        <v>2.1430132389068604</v>
       </c>
       <c r="G3" s="3">
-        <v>1.18</v>
+        <v>1.1825294494628906</v>
       </c>
       <c r="H3" s="4">
-        <v>0.42</v>
+        <v>0.41879957914352417</v>
       </c>
       <c r="I3" s="4">
-        <v>1.36</v>
+        <v>1.3577268123626709</v>
       </c>
       <c r="J3" s="4">
-        <v>1.26</v>
+        <v>1.258309006690979</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -14509,31 +14607,31 @@
         <v>29</v>
       </c>
       <c r="B4" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1053332090377808</v>
       </c>
       <c r="C4" s="3">
-        <v>0.87</v>
+        <v>0.87438958883285522</v>
       </c>
       <c r="D4" s="3">
-        <v>0.73</v>
+        <v>0.7325206995010376</v>
       </c>
       <c r="E4" s="3">
-        <v>0.31</v>
+        <v>0.30922168493270874</v>
       </c>
       <c r="F4" s="3">
-        <v>1.77</v>
+        <v>1.7652401924133301</v>
       </c>
       <c r="G4" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1004093885421753</v>
       </c>
       <c r="H4" s="4">
-        <v>0.31</v>
+        <v>0.31409966945648193</v>
       </c>
       <c r="I4" s="4">
-        <v>0.78</v>
+        <v>0.7753746509552002</v>
       </c>
       <c r="J4" s="4">
-        <v>1.51</v>
+        <v>1.513903021812439</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -14541,31 +14639,31 @@
         <v>30</v>
       </c>
       <c r="B5" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.57669556140899658</v>
       </c>
       <c r="C5" s="3">
-        <v>0.87</v>
+        <v>0.87438958883285522</v>
       </c>
       <c r="D5" s="3">
-        <v>0.77</v>
+        <v>0.77247637510299683</v>
       </c>
       <c r="E5" s="3">
-        <v>0.42</v>
+        <v>0.42372414469718933</v>
       </c>
       <c r="F5" s="3">
-        <v>1.57</v>
+        <v>1.5709018707275391</v>
       </c>
       <c r="G5" s="3">
-        <v>0.49</v>
+        <v>0.48768395185470581</v>
       </c>
       <c r="H5" s="4">
-        <v>0.19</v>
+        <v>0.18845981359481812</v>
       </c>
       <c r="I5" s="4">
-        <v>0.84</v>
+        <v>0.83553707599639893</v>
       </c>
       <c r="J5" s="4">
-        <v>0.77</v>
+        <v>0.76678204536437988</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -14573,31 +14671,31 @@
         <v>31</v>
       </c>
       <c r="B6" s="3">
-        <v>0.46</v>
+        <v>0.45655068755149841</v>
       </c>
       <c r="C6" s="3">
-        <v>0.77</v>
+        <v>0.76509088277816772</v>
       </c>
       <c r="D6" s="3">
-        <v>0.46</v>
+        <v>0.4617595374584198</v>
       </c>
       <c r="E6" s="3">
-        <v>0.17</v>
+        <v>0.16948965191841125</v>
       </c>
       <c r="F6" s="3">
-        <v>1.72</v>
+        <v>1.7237280607223511</v>
       </c>
       <c r="G6" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.55495071411132813</v>
       </c>
       <c r="H6" s="4">
-        <v>0.42</v>
+        <v>0.41879957914352417</v>
       </c>
       <c r="I6" s="4">
-        <v>0.86</v>
+        <v>0.85989367961883545</v>
       </c>
       <c r="J6" s="4">
-        <v>0.87</v>
+        <v>0.86508744955062866</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -14605,31 +14703,31 @@
         <v>32</v>
       </c>
       <c r="B7" s="3">
-        <v>0.44</v>
+        <v>0.44457253813743591</v>
       </c>
       <c r="C7" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.58292639255523682</v>
       </c>
       <c r="D7" s="3">
-        <v>0.34</v>
+        <v>0.335825115442276</v>
       </c>
       <c r="E7" s="3">
-        <v>0.59</v>
+        <v>0.59321379661560059</v>
       </c>
       <c r="F7" s="3">
-        <v>1.48</v>
+        <v>1.4752627611160278</v>
       </c>
       <c r="G7" s="3">
-        <v>0.47</v>
+        <v>0.47086727619171143</v>
       </c>
       <c r="H7" s="4">
-        <v>0.35</v>
+        <v>0.34651708602905273</v>
       </c>
       <c r="I7" s="4">
-        <v>0.81</v>
+        <v>0.81463611125946045</v>
       </c>
       <c r="J7" s="4">
-        <v>0.94</v>
+        <v>0.94373178482055664</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -14637,31 +14735,31 @@
         <v>33</v>
       </c>
       <c r="B8" s="3">
-        <v>0.46</v>
+        <v>0.45655068755149841</v>
       </c>
       <c r="C8" s="3">
-        <v>0.47</v>
+        <v>0.47362768650054932</v>
       </c>
       <c r="D8" s="3">
-        <v>0.45</v>
+        <v>0.44776681065559387</v>
       </c>
       <c r="E8" s="3">
-        <v>0.37</v>
+        <v>0.37106600403785706</v>
       </c>
       <c r="F8" s="3">
-        <v>1.58</v>
+        <v>1.5839662551879883</v>
       </c>
       <c r="G8" s="3">
-        <v>0.39</v>
+        <v>0.38678383827209473</v>
       </c>
       <c r="H8" s="4">
-        <v>0.36</v>
+        <v>0.35597965121269226</v>
       </c>
       <c r="I8" s="4">
-        <v>0.84</v>
+        <v>0.83726489543914795</v>
       </c>
       <c r="J8" s="4">
-        <v>0.83</v>
+        <v>0.82576531171798706</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -14669,31 +14767,31 @@
         <v>34</v>
       </c>
       <c r="B9" s="3">
-        <v>0.66</v>
+        <v>0.65857481956481934</v>
       </c>
       <c r="C9" s="3">
-        <v>0.4</v>
+        <v>0.40076187252998352</v>
       </c>
       <c r="D9" s="3">
-        <v>0.37</v>
+        <v>0.37313216924667358</v>
       </c>
       <c r="E9" s="3">
-        <v>0.25</v>
+        <v>0.24737733602523804</v>
       </c>
       <c r="F9" s="3">
-        <v>1.26</v>
+        <v>1.2556016445159912</v>
       </c>
       <c r="G9" s="3">
-        <v>0.33</v>
+        <v>0.33305755257606506</v>
       </c>
       <c r="H9" s="4">
-        <v>0.5</v>
+        <v>0.49811831116676331</v>
       </c>
       <c r="I9" s="4">
-        <v>0.54</v>
+        <v>0.54309076070785522</v>
       </c>
       <c r="J9" s="4">
-        <v>0.56999999999999995</v>
+        <v>0.56818699836730957</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -14701,31 +14799,31 @@
         <v>35</v>
       </c>
       <c r="B10" s="3">
-        <v>0.76</v>
+        <v>0.75608879327774048</v>
       </c>
       <c r="C10" s="3">
-        <v>0.26</v>
+        <v>0.25520727038383484</v>
       </c>
       <c r="D10" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29021391272544861</v>
       </c>
       <c r="E10" s="3">
-        <v>0.25</v>
+        <v>0.24737733602523804</v>
       </c>
       <c r="F10" s="3">
-        <v>1.42</v>
+        <v>1.4205218553543091</v>
       </c>
       <c r="G10" s="3">
-        <v>0.35</v>
+        <v>0.35315045714378357</v>
       </c>
       <c r="H10" s="4">
-        <v>0.08</v>
+        <v>8.3759918808937073E-2</v>
       </c>
       <c r="I10" s="4">
-        <v>0.75</v>
+        <v>0.74674975872039795</v>
       </c>
       <c r="J10" s="4">
-        <v>0.56999999999999995</v>
+        <v>0.5701712965965271</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -14733,31 +14831,31 @@
         <v>36</v>
       </c>
       <c r="B11" s="3">
-        <v>0.5</v>
+        <v>0.5046086311340332</v>
       </c>
       <c r="C11" s="3">
-        <v>0.38</v>
+        <v>0.38254544138908386</v>
       </c>
       <c r="D11" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.55315732955932617</v>
       </c>
       <c r="E11" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1131980419158936</v>
       </c>
       <c r="F11" s="3">
-        <v>1.88</v>
+        <v>1.884222149848938</v>
       </c>
       <c r="G11" s="3">
-        <v>0.44</v>
+        <v>0.43823361396789551</v>
       </c>
       <c r="H11" s="4">
-        <v>0.19</v>
+        <v>0.19491586089134216</v>
       </c>
       <c r="I11" s="4">
-        <v>1.35</v>
+        <v>1.3528138399124146</v>
       </c>
       <c r="J11" s="4">
-        <v>0.51</v>
+        <v>0.50730985403060913</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -14765,31 +14863,31 @@
         <v>37</v>
       </c>
       <c r="B12" s="3">
-        <v>1.89</v>
+        <v>1.8934025764465332</v>
       </c>
       <c r="C12" s="3">
-        <v>0.95</v>
+        <v>0.9523242712020874</v>
       </c>
       <c r="D12" s="3">
-        <v>1</v>
+        <v>1.0044173002243042</v>
       </c>
       <c r="E12" s="3">
-        <v>2.23</v>
+        <v>2.2263960838317871</v>
       </c>
       <c r="F12" s="3">
-        <v>2.59</v>
+        <v>2.5933566093444824</v>
       </c>
       <c r="G12" s="3">
-        <v>0.77</v>
+        <v>0.77356767654418945</v>
       </c>
       <c r="H12" s="4">
-        <v>0.24</v>
+        <v>0.23823049664497375</v>
       </c>
       <c r="I12" s="4">
-        <v>2.44</v>
+        <v>2.4436049461364746</v>
       </c>
       <c r="J12" s="4">
-        <v>1.06</v>
+        <v>1.0616981983184814</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -14797,31 +14895,31 @@
         <v>38</v>
       </c>
       <c r="B13" s="3">
-        <v>1.32</v>
+        <v>1.3215939998626709</v>
       </c>
       <c r="C13" s="3">
-        <v>0.93</v>
+        <v>0.92903894186019897</v>
       </c>
       <c r="D13" s="3">
-        <v>1.81</v>
+        <v>1.805039644241333</v>
       </c>
       <c r="E13" s="3">
-        <v>4.3899999999999997</v>
+        <v>4.3909478187561035</v>
       </c>
       <c r="F13" s="3">
-        <v>4.18</v>
+        <v>4.1773228645324707</v>
       </c>
       <c r="G13" s="3">
-        <v>0.67</v>
+        <v>0.67266756296157837</v>
       </c>
       <c r="H13" s="4">
-        <v>0.54</v>
+        <v>0.54143291711807251</v>
       </c>
       <c r="I13" s="4">
-        <v>3.67</v>
+        <v>3.6658625602722168</v>
       </c>
       <c r="J13" s="4">
-        <v>2.95</v>
+        <v>2.9491617679595947</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -14829,31 +14927,31 @@
         <v>39</v>
       </c>
       <c r="B14" s="3">
-        <v>2.21</v>
+        <v>2.2106664180755615</v>
       </c>
       <c r="C14" s="3">
-        <v>1.06</v>
+        <v>1.0565540790557861</v>
       </c>
       <c r="D14" s="3">
-        <v>2.4300000000000002</v>
+        <v>2.430980920791626</v>
       </c>
       <c r="E14" s="3">
-        <v>7.79</v>
+        <v>7.7923860549926758</v>
       </c>
       <c r="F14" s="3">
-        <v>5.33</v>
+        <v>5.326474666595459</v>
       </c>
       <c r="G14" s="3">
-        <v>1.28</v>
+        <v>1.2780683040618896</v>
       </c>
       <c r="H14" s="4">
-        <v>0.73</v>
+        <v>0.7328992486000061</v>
       </c>
       <c r="I14" s="4">
-        <v>5.45</v>
+        <v>5.4535360336303711</v>
       </c>
       <c r="J14" s="4">
-        <v>4.25</v>
+        <v>4.2467927932739258</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -14861,31 +14959,31 @@
         <v>40</v>
       </c>
       <c r="B15" s="3">
-        <v>2.67</v>
+        <v>2.6672170162200928</v>
       </c>
       <c r="C15" s="3">
-        <v>1.68</v>
+        <v>1.6804071664810181</v>
       </c>
       <c r="D15" s="3">
-        <v>1.78</v>
+        <v>1.7770745754241943</v>
       </c>
       <c r="E15" s="3">
-        <v>10.76</v>
+        <v>10.760913848876953</v>
       </c>
       <c r="F15" s="3">
-        <v>7.11</v>
+        <v>7.1123189926147461</v>
       </c>
       <c r="G15" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1267181634902954</v>
       </c>
       <c r="H15" s="4">
-        <v>0.95</v>
+        <v>0.95292198657989502</v>
       </c>
       <c r="I15" s="4">
-        <v>5.5</v>
+        <v>5.4987936019897461</v>
       </c>
       <c r="J15" s="4">
-        <v>5.45</v>
+        <v>5.4461188316345215</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -14893,31 +14991,31 @@
         <v>41</v>
       </c>
       <c r="B16" s="3">
-        <v>4.5599999999999996</v>
+        <v>4.5551424026489258</v>
       </c>
       <c r="C16" s="3">
-        <v>2.3199999999999998</v>
+        <v>2.3202061653137207</v>
       </c>
       <c r="D16" s="3">
-        <v>2.81</v>
+        <v>2.8088922500610352</v>
       </c>
       <c r="E16" s="3">
-        <v>12.25</v>
+        <v>12.24517822265625</v>
       </c>
       <c r="F16" s="3">
-        <v>12.05</v>
+        <v>12.050566673278809</v>
       </c>
       <c r="G16" s="3">
-        <v>2.33</v>
+        <v>2.3322110176086426</v>
       </c>
       <c r="H16" s="4">
-        <v>1.7</v>
+        <v>1.6961382627487183</v>
       </c>
       <c r="I16" s="4">
-        <v>6.36</v>
+        <v>6.3612508773803711</v>
       </c>
       <c r="J16" s="4">
-        <v>8.73</v>
+        <v>8.7300834655761719</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -14925,31 +15023,31 @@
         <v>42</v>
       </c>
       <c r="B17" s="3">
-        <v>8.67</v>
+        <v>8.6712350845336914</v>
       </c>
       <c r="C17" s="3">
-        <v>3.62</v>
+        <v>3.6225960254669189</v>
       </c>
       <c r="D17" s="3">
-        <v>3.44</v>
+        <v>3.4353981018066406</v>
       </c>
       <c r="E17" s="3">
-        <v>16.88</v>
+        <v>16.883502960205078</v>
       </c>
       <c r="F17" s="3">
-        <v>16.43</v>
+        <v>16.429767608642578</v>
       </c>
       <c r="G17" s="3">
-        <v>3.04</v>
+        <v>3.0384438037872314</v>
       </c>
       <c r="H17" s="4">
-        <v>3.06</v>
+        <v>3.057236909866333</v>
       </c>
       <c r="I17" s="4">
-        <v>7.83</v>
+        <v>7.8343825340270996</v>
       </c>
       <c r="J17" s="4">
-        <v>11.91</v>
+        <v>11.909671783447266</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -14957,31 +15055,31 @@
         <v>43</v>
       </c>
       <c r="B18" s="3">
-        <v>13.88</v>
+        <v>13.884951591491699</v>
       </c>
       <c r="C18" s="3">
-        <v>4.4800000000000004</v>
+        <v>4.4798507690429688</v>
       </c>
       <c r="D18" s="3">
-        <v>6</v>
+        <v>5.9682765007019043</v>
       </c>
       <c r="E18" s="3">
-        <v>17.440000000000001</v>
+        <v>17.440101623535156</v>
       </c>
       <c r="F18" s="3">
-        <v>19.350000000000001</v>
+        <v>19.349235534667969</v>
       </c>
       <c r="G18" s="3">
-        <v>5.21</v>
+        <v>5.2064146995544434</v>
       </c>
       <c r="H18" s="4">
-        <v>4.59</v>
+        <v>4.5862536430358887</v>
       </c>
       <c r="I18" s="4">
-        <v>11.41</v>
+        <v>11.405611038208008</v>
       </c>
       <c r="J18" s="4">
-        <v>18.010000000000002</v>
+        <v>18.011541366577148</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -14989,31 +15087,31 @@
         <v>44</v>
       </c>
       <c r="B19" s="3">
-        <v>16.52</v>
+        <v>16.519250869750977</v>
       </c>
       <c r="C19" s="3">
-        <v>7.25</v>
+        <v>7.251431941986084</v>
       </c>
       <c r="D19" s="3">
-        <v>8.34</v>
+        <v>8.3410301208496094</v>
       </c>
       <c r="E19" s="3">
-        <v>24.43</v>
+        <v>24.428512573242188</v>
       </c>
       <c r="F19" s="3">
-        <v>21.94</v>
+        <v>21.942592620849609</v>
       </c>
       <c r="G19" s="3">
-        <v>5.82</v>
+        <v>5.8185739517211914</v>
       </c>
       <c r="H19" s="4">
-        <v>7.52</v>
+        <v>7.515289306640625</v>
       </c>
       <c r="I19" s="4">
-        <v>18.170000000000002</v>
+        <v>18.168624877929688</v>
       </c>
       <c r="J19" s="4">
-        <v>21.96</v>
+        <v>21.963052749633789</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -15021,31 +15119,31 @@
         <v>45</v>
       </c>
       <c r="B20" s="3">
-        <v>20.85</v>
+        <v>20.854867935180664</v>
       </c>
       <c r="C20" s="3">
-        <v>7.79</v>
+        <v>7.8111362457275391</v>
       </c>
       <c r="D20" s="3">
-        <v>7.02</v>
+        <v>7.0243420600891113</v>
       </c>
       <c r="E20" s="3">
-        <v>26.53</v>
+        <v>26.531219482421875</v>
       </c>
       <c r="F20" s="3">
-        <v>19.55</v>
+        <v>19.551113128662109</v>
       </c>
       <c r="G20" s="3">
-        <v>7.08</v>
+        <v>7.0798258781433105</v>
       </c>
       <c r="H20" s="4">
-        <v>12.04</v>
+        <v>12.043732643127441</v>
       </c>
       <c r="I20" s="4">
-        <v>17.71</v>
+        <v>17.713386535644531</v>
       </c>
       <c r="J20" s="4">
-        <v>23.08</v>
+        <v>23.084178924560547</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -15053,46 +15151,64 @@
         <v>46</v>
       </c>
       <c r="B21" s="3">
-        <v>24.64</v>
+        <v>24.66911506652832</v>
       </c>
       <c r="C21" s="3">
-        <v>9.7100000000000009</v>
+        <v>9.8661308288574219</v>
       </c>
       <c r="D21" s="3">
-        <v>7.78</v>
+        <v>8.0458097457885742</v>
       </c>
       <c r="E21" s="3">
-        <v>26.1</v>
+        <v>26.098308563232422</v>
       </c>
       <c r="F21" s="3">
-        <v>20.64</v>
+        <v>20.638149261474609</v>
       </c>
       <c r="G21" s="3">
-        <v>8.9600000000000009</v>
+        <v>8.9632949829101563</v>
       </c>
       <c r="H21" s="4">
-        <v>15.47</v>
+        <v>15.473788261413574</v>
       </c>
       <c r="I21" s="4">
-        <v>21.05</v>
+        <v>21.762172698974609</v>
       </c>
       <c r="J21" s="4">
-        <v>29.41</v>
+        <v>29.406597137451172</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>47</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="B22" s="3">
+        <v>19.45539665222168</v>
+      </c>
+      <c r="C22" s="3">
+        <v>9.6569547653198242</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10.682635307312012</v>
+      </c>
+      <c r="E22" s="3">
+        <v>30.056346893310547</v>
+      </c>
+      <c r="F22" s="3">
+        <v>14.876859664916992</v>
+      </c>
+      <c r="G22" s="3">
+        <v>9.7032289505004883</v>
+      </c>
+      <c r="H22" s="4">
+        <v>16.861225128173828</v>
+      </c>
+      <c r="I22" s="4">
+        <v>21.832464218139648</v>
+      </c>
+      <c r="J22" s="4">
+        <v>22.882007598876953</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -15506,7 +15622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15551,31 +15667,31 @@
         <v>27</v>
       </c>
       <c r="B2" s="3">
-        <v>0.13</v>
+        <v>0.13075663149356842</v>
       </c>
       <c r="C2" s="3">
-        <v>0.16</v>
+        <v>0.15705062448978424</v>
       </c>
       <c r="D2" s="3">
-        <v>0.12</v>
+        <v>0.11986702680587769</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3">
-        <v>0.19</v>
+        <v>0.19477562606334686</v>
       </c>
       <c r="G2" s="3">
-        <v>0.02</v>
+        <v>1.7103113234043121E-2</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
       </c>
       <c r="I2" s="4">
-        <v>0.23</v>
+        <v>0.22964039444923401</v>
       </c>
       <c r="J2" s="4">
-        <v>0.06</v>
+        <v>6.0877177864313126E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -15583,31 +15699,31 @@
         <v>28</v>
       </c>
       <c r="B3" s="3">
-        <v>0.05</v>
+        <v>5.2302651107311249E-2</v>
       </c>
       <c r="C3" s="3">
-        <v>0.12</v>
+        <v>0.12340131402015686</v>
       </c>
       <c r="D3" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.14312003552913666</v>
       </c>
       <c r="E3" s="3">
-        <v>0.08</v>
+        <v>8.4744825959205627E-2</v>
       </c>
       <c r="F3" s="3">
-        <v>0.02</v>
+        <v>2.1423524245619774E-2</v>
       </c>
       <c r="G3" s="3">
-        <v>0.03</v>
+        <v>3.2848041504621506E-2</v>
       </c>
       <c r="H3" s="4">
-        <v>0.02</v>
+        <v>2.0939979702234268E-2</v>
       </c>
       <c r="I3" s="4">
-        <v>0.2</v>
+        <v>0.2041248083114624</v>
       </c>
       <c r="J3" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.28409349918365479</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -15615,31 +15731,31 @@
         <v>29</v>
       </c>
       <c r="B4" s="3">
-        <v>0.15</v>
+        <v>0.1512177586555481</v>
       </c>
       <c r="C4" s="3">
-        <v>0.06</v>
+        <v>5.8893982321023941E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>0.04</v>
+        <v>3.9955675601959229E-2</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>0.15</v>
+        <v>0.14935484528541565</v>
       </c>
       <c r="G4" s="3">
-        <v>0.02</v>
+        <v>1.7103113234043121E-2</v>
       </c>
       <c r="H4" s="4">
-        <v>0.02</v>
+        <v>2.0939979702234268E-2</v>
       </c>
       <c r="I4" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.14097721874713898</v>
       </c>
       <c r="J4" s="4">
-        <v>0.1</v>
+        <v>0.10146196186542511</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -15647,31 +15763,31 @@
         <v>30</v>
       </c>
       <c r="B5" s="3">
-        <v>0.02</v>
+        <v>2.402898296713829E-2</v>
       </c>
       <c r="C5" s="3">
-        <v>0.02</v>
+        <v>1.963132806122303E-2</v>
       </c>
       <c r="D5" s="3">
-        <v>0.1</v>
+        <v>0.10018402338027954</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>0.13</v>
+        <v>0.12955892086029053</v>
       </c>
       <c r="G5" s="3">
-        <v>0.02</v>
+        <v>1.9665028899908066E-2</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>0.13</v>
+        <v>0.1339210718870163</v>
       </c>
       <c r="J5" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.13762754201889038</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -15679,31 +15795,31 @@
         <v>31</v>
       </c>
       <c r="B6" s="3">
-        <v>0.05</v>
+        <v>5.4881233721971512E-2</v>
       </c>
       <c r="C6" s="3">
-        <v>0.02</v>
+        <v>1.963132806122303E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>0.17</v>
+        <v>0.1660277396440506</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>0.12</v>
+        <v>0.11775144934654236</v>
       </c>
       <c r="G6" s="3">
-        <v>0.02</v>
+        <v>1.752934418618679E-2</v>
       </c>
       <c r="H6" s="4">
-        <v>0.04</v>
+        <v>4.1879959404468536E-2</v>
       </c>
       <c r="I6" s="4">
-        <v>0.16</v>
+        <v>0.15840145945549011</v>
       </c>
       <c r="J6" s="4">
-        <v>0.06</v>
+        <v>6.0877177864313126E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -15711,31 +15827,31 @@
         <v>32</v>
       </c>
       <c r="B7" s="3">
-        <v>0.06</v>
+        <v>6.0487102717161179E-2</v>
       </c>
       <c r="C7" s="3">
-        <v>0.04</v>
+        <v>3.6432899534702301E-2</v>
       </c>
       <c r="D7" s="3">
-        <v>0.03</v>
+        <v>2.7985425665974617E-2</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>0.17</v>
+        <v>0.16821636259555817</v>
       </c>
       <c r="G7" s="3">
-        <v>0.02</v>
+        <v>1.9665028899908066E-2</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <v>0.2</v>
+        <v>0.20365902781486511</v>
       </c>
       <c r="J7" s="4">
-        <v>0.06</v>
+        <v>6.0877177864313126E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -15743,31 +15859,31 @@
         <v>33</v>
       </c>
       <c r="B8" s="3">
-        <v>0.12</v>
+        <v>0.12097420543432236</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0.03</v>
+        <v>2.7985425665974617E-2</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <v>0.13</v>
+        <v>0.12854114174842834</v>
       </c>
       <c r="G8" s="3">
-        <v>0.02</v>
+        <v>1.752934418618679E-2</v>
       </c>
       <c r="H8" s="4">
-        <v>0.02</v>
+        <v>2.0939979702234268E-2</v>
       </c>
       <c r="I8" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>6.7886345088481903E-2</v>
       </c>
       <c r="J8" s="4">
-        <v>0.08</v>
+        <v>7.8644312918186188E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -15775,31 +15891,31 @@
         <v>34</v>
       </c>
       <c r="B9" s="3">
-        <v>0.1</v>
+        <v>0.1046053022146225</v>
       </c>
       <c r="C9" s="3">
-        <v>0.1</v>
+        <v>9.8156638443470001E-2</v>
       </c>
       <c r="D9" s="3">
-        <v>0.11</v>
+        <v>0.11194170266389847</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>0.17</v>
+        <v>0.17151154577732086</v>
       </c>
       <c r="G9" s="3">
-        <v>0.02</v>
+        <v>1.9665028899908066E-2</v>
       </c>
       <c r="H9" s="4">
-        <v>0.06</v>
+        <v>6.4971953630447388E-2</v>
       </c>
       <c r="I9" s="4">
-        <v>0.02</v>
+        <v>2.2628780454397202E-2</v>
       </c>
       <c r="J9" s="4">
-        <v>0.08</v>
+        <v>8.1169575452804565E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -15807,31 +15923,31 @@
         <v>35</v>
       </c>
       <c r="B10" s="3">
-        <v>0.06</v>
+        <v>6.0487102717161179E-2</v>
       </c>
       <c r="C10" s="3">
-        <v>0.04</v>
+        <v>3.926265612244606E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>0.1</v>
+        <v>9.6737965941429138E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>0.05</v>
+        <v>5.3836699575185776E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2847269475460052E-2</v>
       </c>
       <c r="G10" s="3">
-        <v>0.02</v>
+        <v>1.8772562965750694E-2</v>
       </c>
       <c r="H10" s="4">
-        <v>0.06</v>
+        <v>6.2819935381412506E-2</v>
       </c>
       <c r="I10" s="4">
-        <v>0.08</v>
+        <v>7.6546803116798401E-2</v>
       </c>
       <c r="J10" s="4">
-        <v>0.12</v>
+        <v>0.12175435572862625</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -15845,25 +15961,25 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>0.05</v>
+        <v>4.7255426645278931E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>0.08</v>
+        <v>8.4744825959205627E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>0.19</v>
+        <v>0.1850380003452301</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11" s="4">
-        <v>0.02</v>
+        <v>2.1657317876815796E-2</v>
       </c>
       <c r="I11" s="4">
-        <v>0.16</v>
+        <v>0.16327063739299774</v>
       </c>
       <c r="J11" s="4">
-        <v>0.08</v>
+        <v>8.1169575452804565E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -15871,31 +15987,31 @@
         <v>37</v>
       </c>
       <c r="B12" s="3">
-        <v>0.19</v>
+        <v>0.19208431243896484</v>
       </c>
       <c r="C12" s="3">
-        <v>0.04</v>
+        <v>4.4017631560564041E-2</v>
       </c>
       <c r="D12" s="3">
-        <v>0.15</v>
+        <v>0.15211443603038788</v>
       </c>
       <c r="E12" s="3">
-        <v>0.05</v>
+        <v>5.3836699575185776E-2</v>
       </c>
       <c r="F12" s="3">
-        <v>0.24</v>
+        <v>0.23819261789321899</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
       </c>
       <c r="H12" s="4">
-        <v>0.02</v>
+        <v>2.1657317876815796E-2</v>
       </c>
       <c r="I12" s="4">
-        <v>0.26</v>
+        <v>0.25845822691917419</v>
       </c>
       <c r="J12" s="4">
-        <v>0.16</v>
+        <v>0.16233915090560913</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -15903,31 +16019,31 @@
         <v>38</v>
       </c>
       <c r="B13" s="3">
-        <v>0.16</v>
+        <v>0.15690794587135315</v>
       </c>
       <c r="C13" s="3">
-        <v>0.08</v>
+        <v>8.2267537713050842E-2</v>
       </c>
       <c r="D13" s="3">
-        <v>0.36</v>
+        <v>0.36391928791999817</v>
       </c>
       <c r="E13" s="3">
-        <v>0.48</v>
+        <v>0.48453029990196228</v>
       </c>
       <c r="F13" s="3">
-        <v>0.32</v>
+        <v>0.3203335702419281</v>
       </c>
       <c r="G13" s="3">
-        <v>0.06</v>
+        <v>5.5492110550403595E-2</v>
       </c>
       <c r="H13" s="4">
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>0.61</v>
+        <v>0.61097711324691772</v>
       </c>
       <c r="J13" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.27525508403778076</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -15935,31 +16051,31 @@
         <v>39</v>
       </c>
       <c r="B14" s="3">
-        <v>0.33</v>
+        <v>0.33267906308174133</v>
       </c>
       <c r="C14" s="3">
-        <v>0.11</v>
+        <v>0.1092986986041069</v>
       </c>
       <c r="D14" s="3">
-        <v>0.45</v>
+        <v>0.45125991106033325</v>
       </c>
       <c r="E14" s="3">
-        <v>0.48</v>
+        <v>0.47942420840263367</v>
       </c>
       <c r="F14" s="3">
-        <v>0.61</v>
+        <v>0.60563415288925171</v>
       </c>
       <c r="G14" s="3">
-        <v>0.09</v>
+        <v>9.3862816691398621E-2</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>1.06</v>
+        <v>1.0635527372360229</v>
       </c>
       <c r="J14" s="4">
-        <v>0.35</v>
+        <v>0.35389941930770874</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -15967,31 +16083,31 @@
         <v>40</v>
       </c>
       <c r="B15" s="3">
-        <v>0.11</v>
+        <v>0.10976246744394302</v>
       </c>
       <c r="C15" s="3">
-        <v>0.36</v>
+        <v>0.3644256591796875</v>
       </c>
       <c r="D15" s="3">
-        <v>0.33</v>
+        <v>0.33436283469200134</v>
       </c>
       <c r="E15" s="3">
-        <v>0.61</v>
+        <v>0.61017626523971558</v>
       </c>
       <c r="F15" s="3">
-        <v>0.65</v>
+        <v>0.64779460430145264</v>
       </c>
       <c r="G15" s="3">
-        <v>0.17</v>
+        <v>0.16895307600498199</v>
       </c>
       <c r="H15" s="4">
-        <v>0.04</v>
+        <v>4.3314635753631592E-2</v>
       </c>
       <c r="I15" s="4">
-        <v>0.86</v>
+        <v>0.85989367961883545</v>
       </c>
       <c r="J15" s="4">
-        <v>0.53</v>
+        <v>0.53084909915924072</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -15999,31 +16115,31 @@
         <v>41</v>
       </c>
       <c r="B16" s="3">
-        <v>0.45</v>
+        <v>0.45365327596664429</v>
       </c>
       <c r="C16" s="3">
-        <v>0.36</v>
+        <v>0.35840582847595215</v>
       </c>
       <c r="D16" s="3">
-        <v>0.32</v>
+        <v>0.32335537672042847</v>
       </c>
       <c r="E16" s="3">
-        <v>0.44</v>
+        <v>0.4358401894569397</v>
       </c>
       <c r="F16" s="3">
-        <v>0.76</v>
+        <v>0.76115864515304565</v>
       </c>
       <c r="G16" s="3">
-        <v>0.11</v>
+        <v>0.10814039409160614</v>
       </c>
       <c r="H16" s="4">
-        <v>0.15</v>
+        <v>0.15160122513771057</v>
       </c>
       <c r="I16" s="4">
-        <v>0.69</v>
+        <v>0.6919255256652832</v>
       </c>
       <c r="J16" s="4">
-        <v>0.92</v>
+        <v>0.91895616054534912</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -16031,31 +16147,31 @@
         <v>42</v>
       </c>
       <c r="B17" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.57462745904922485</v>
       </c>
       <c r="C17" s="3">
-        <v>0.31</v>
+        <v>0.3063887357711792</v>
       </c>
       <c r="D17" s="3">
-        <v>0.49</v>
+        <v>0.49493023753166199</v>
       </c>
       <c r="E17" s="3">
-        <v>0.92</v>
+        <v>0.91526436805725098</v>
       </c>
       <c r="F17" s="3">
-        <v>0.85</v>
+        <v>0.85409945249557495</v>
       </c>
       <c r="G17" s="3">
-        <v>0.21</v>
+        <v>0.20831501483917236</v>
       </c>
       <c r="H17" s="4">
-        <v>0.27</v>
+        <v>0.27221971750259399</v>
       </c>
       <c r="I17" s="4">
-        <v>0.89</v>
+        <v>0.89280712604522705</v>
       </c>
       <c r="J17" s="4">
-        <v>0.87</v>
+        <v>0.87076354026794434</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -16063,31 +16179,31 @@
         <v>43</v>
       </c>
       <c r="B18" s="3">
-        <v>0.91</v>
+        <v>0.9055403470993042</v>
       </c>
       <c r="C18" s="3">
-        <v>0.33</v>
+        <v>0.33119520545005798</v>
       </c>
       <c r="D18" s="3">
-        <v>0.66</v>
+        <v>0.65505474805831909</v>
       </c>
       <c r="E18" s="3">
-        <v>0.7</v>
+        <v>0.69734430313110352</v>
       </c>
       <c r="F18" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1273124217987061</v>
       </c>
       <c r="G18" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.28695294260978699</v>
       </c>
       <c r="H18" s="4">
-        <v>0.18</v>
+        <v>0.17888219654560089</v>
       </c>
       <c r="I18" s="4">
-        <v>1.32</v>
+        <v>1.3168904781341553</v>
       </c>
       <c r="J18" s="4">
-        <v>1.1499999999999999</v>
+        <v>1.1547081470489502</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -16095,31 +16211,31 @@
         <v>44</v>
       </c>
       <c r="B19" s="3">
-        <v>1.45</v>
+        <v>1.4543526172637939</v>
       </c>
       <c r="C19" s="3">
-        <v>0.63</v>
+        <v>0.62752777338027954</v>
       </c>
       <c r="D19" s="3">
-        <v>0.92</v>
+        <v>0.91707664728164673</v>
       </c>
       <c r="E19" s="3">
-        <v>0.92</v>
+        <v>0.91526436805725098</v>
       </c>
       <c r="F19" s="3">
-        <v>0.95</v>
+        <v>0.94727396965026855</v>
       </c>
       <c r="G19" s="3">
-        <v>0.3</v>
+        <v>0.30270040035247803</v>
       </c>
       <c r="H19" s="4">
-        <v>0.42</v>
+        <v>0.41739180684089661</v>
       </c>
       <c r="I19" s="4">
-        <v>1.61</v>
+        <v>1.6070528030395508</v>
       </c>
       <c r="J19" s="4">
-        <v>1.42</v>
+        <v>1.4151924848556519</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -16127,31 +16243,31 @@
         <v>45</v>
       </c>
       <c r="B20" s="3">
-        <v>1.65</v>
+        <v>1.6464369297027588</v>
       </c>
       <c r="C20" s="3">
-        <v>0.75</v>
+        <v>0.74954706430435181</v>
       </c>
       <c r="D20" s="3">
-        <v>0.92</v>
+        <v>0.92269307374954224</v>
       </c>
       <c r="E20" s="3">
-        <v>1.44</v>
+        <v>1.4382725954055786</v>
       </c>
       <c r="F20" s="3">
-        <v>0.89</v>
+        <v>0.88515764474868774</v>
       </c>
       <c r="G20" s="3">
-        <v>0.43</v>
+        <v>0.43263065814971924</v>
       </c>
       <c r="H20" s="4">
-        <v>0.52</v>
+        <v>0.52028924226760864</v>
       </c>
       <c r="I20" s="4">
-        <v>1.79</v>
+        <v>1.7856142520904541</v>
       </c>
       <c r="J20" s="4">
-        <v>1.25</v>
+        <v>1.2493563890457153</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -16159,46 +16275,64 @@
         <v>46</v>
       </c>
       <c r="B21" s="3">
-        <v>1.73</v>
+        <v>1.7287588119506836</v>
       </c>
       <c r="C21" s="3">
-        <v>1.75</v>
+        <v>0.74954706430435181</v>
       </c>
       <c r="D21" s="3">
-        <v>0.63</v>
+        <v>0.65765750408172607</v>
       </c>
       <c r="E21" s="3">
-        <v>1.26</v>
+        <v>1.2639365196228027</v>
       </c>
       <c r="F21" s="3">
-        <v>1.32</v>
+        <v>1.335500955581665</v>
       </c>
       <c r="G21" s="3">
-        <v>0.65</v>
+        <v>0.6485857367515564</v>
       </c>
       <c r="H21" s="4">
-        <v>0.66</v>
+        <v>0.65590143203735352</v>
       </c>
       <c r="I21" s="4">
-        <v>1.52</v>
+        <v>1.5177720785140991</v>
       </c>
       <c r="J21" s="4">
-        <v>1.45</v>
+        <v>1.4519506692886353</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>47</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="B22" s="3">
+        <v>1.7287588119506836</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.76697838306427002</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.90952634811401367</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.3511046171188354</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.55779355764389038</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.57176738977432251</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.59736913442611694</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.9238219261169434</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1.173637866973877</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -16611,7 +16745,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16626,7 +16760,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16640,8 +16774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3D97F0-2300-4E4D-BA55-520B52BE6BA3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16656,7 +16790,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>